<commit_message>
Modified .xlsx file and Readme.md
</commit_message>
<xml_diff>
--- a/Formulas_and_Templates/Templates/Distribution/Binomial_Distribution/Binomial_Distribution.xlsx
+++ b/Formulas_and_Templates/Templates/Distribution/Binomial_Distribution/Binomial_Distribution.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\DADS\GitHub_Repositories\Excel\Formulas_and_Templates\Templates\Distribution\Binomial_Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{095236AC-886C-4755-8873-BC9EF118B4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC0385B-263B-4CA4-B7F6-B2D15431A061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11736" yWindow="150" windowWidth="10782" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11688" yWindow="0" windowWidth="10782" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binomial" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -345,67 +345,67 @@
                 <c:formatCode>0.0000000%</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.8124545836334979E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.9518741669899233E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>9.9845870849869164E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.2257896736111576E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7.3820955992255327E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.12719918570973221</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.17122967307079331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.18440118638393124</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.16135103808593984</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.11584177093349528</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>6.8613972014454891E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3.3587259028054817E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1.3564085376714463E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>4.4946081721657337E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1.2100868155830826E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2.6063408335635669E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>4.3856696718617628E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5.5565045616348105E-6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>4.9866066578773876E-7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2.8264167291612782E-8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>7.609583501588035E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1199,7 +1199,9 @@
   <autoFilter ref="A4:B25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Successes"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Percentage of Outcomes" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Percentage of Outcomes" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>_xlfn.BINOM.DIST(A5,$B$2,$B$1,FALSE)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1530,7 +1532,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1572,7 +1574,8 @@
         <v>0</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <f t="shared" ref="B5:B25" si="0">_xlfn.BINOM.DIST(A5,$B$2,$B$1,FALSE)</f>
+        <v>1.8124545836334979E-4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1580,7 +1583,8 @@
         <v>1</v>
       </c>
       <c r="B6" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.9518741669899233E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1588,7 +1592,8 @@
         <v>2</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9845870849869164E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1596,7 +1601,8 @@
         <v>3</v>
       </c>
       <c r="B8" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.2257896736111576E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1604,7 +1610,8 @@
         <v>4</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.3820955992255327E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1612,7 +1619,8 @@
         <v>5</v>
       </c>
       <c r="B10" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.12719918570973221</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1620,7 +1628,8 @@
         <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.17122967307079331</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1628,7 +1637,8 @@
         <v>7</v>
       </c>
       <c r="B12" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.18440118638393124</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1636,7 +1646,8 @@
         <v>8</v>
       </c>
       <c r="B13" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16135103808593984</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1644,7 +1655,8 @@
         <v>9</v>
       </c>
       <c r="B14" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.11584177093349528</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1652,7 +1664,8 @@
         <v>10</v>
       </c>
       <c r="B15" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.8613972014454891E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1660,7 +1673,8 @@
         <v>11</v>
       </c>
       <c r="B16" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.3587259028054817E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1668,7 +1682,8 @@
         <v>12</v>
       </c>
       <c r="B17" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3564085376714463E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1676,7 +1691,8 @@
         <v>13</v>
       </c>
       <c r="B18" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.4946081721657337E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1684,7 +1700,8 @@
         <v>14</v>
       </c>
       <c r="B19" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.2100868155830826E-3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1692,7 +1709,8 @@
         <v>15</v>
       </c>
       <c r="B20" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6063408335635669E-4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1700,7 +1718,8 @@
         <v>16</v>
       </c>
       <c r="B21" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.3856696718617628E-5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1708,7 +1727,8 @@
         <v>17</v>
       </c>
       <c r="B22" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.5565045616348105E-6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1716,7 +1736,8 @@
         <v>18</v>
       </c>
       <c r="B23" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.9866066578773876E-7</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1724,7 +1745,8 @@
         <v>19</v>
       </c>
       <c r="B24" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.8264167291612782E-8</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1732,7 +1754,8 @@
         <v>20</v>
       </c>
       <c r="B25" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.609583501588035E-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>